<commit_message>
refactoring Koans and Art Gallery
</commit_message>
<xml_diff>
--- a/3-database-driven-applications/exercises/mvc/ArtGallery/ArtGallery.xlsx
+++ b/3-database-driven-applications/exercises/mvc/ArtGallery/ArtGallery.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynn\Documents\GitHub\csharp-dotnet-milestones\3-database-driven-applications\exercises\mvc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lynn\Documents\GitHub\csharp-dotnet-milestones\3-database-driven-applications\exercises\mvc\ArtGallery\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22812" windowHeight="8796" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22812" windowHeight="8796" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="391">
   <si>
     <t>Image</t>
   </si>
@@ -1017,6 +1017,201 @@
   <si>
     <t>Penguin, Golden Eagle, Batroc</t>
   </si>
+  <si>
+    <t>https://cdn1.artstation.com/p/assets/images/images/001/622/077/large/alex-andreev-pilots-1200.jpg?1449657939</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/35054/Images/Large_DSCF1548.jpg</t>
+  </si>
+  <si>
+    <t>https://s-media-cache-ak0.pinimg.com/736x/4e/b7/b3/4eb7b3703c25663f4b94b1019b0dc90e.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/35894/Images/Large_KMUgallery_heart.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/41653/Images/Large_Tumacacori_Mission_(1500x1090).jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/44537/Images/Large_sam6479-version4.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/43710/Images/Large_1.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/28028/Images/Large_IMG-4897-cropped.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/45291/Images/Large_mistersteethchatteredindiainkoncutpaper12.5x152013.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/43166/Images/Large_Melanie_Duault04.jpg</t>
+  </si>
+  <si>
+    <t>https://nerskine.files.wordpress.com/2012/11/winter-field-ii-18x18-oil-on-canvas-2015.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/41931/Images/Large_P1030476.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/41416/Images/Large_1.__Layered_Landscape.jpg</t>
+  </si>
+  <si>
+    <t>http://saimg-a.akamaihd.net/saatchi/403041/art/3132944/2202835-TEWCTIPU-7.jpg</t>
+  </si>
+  <si>
+    <t>http://www.ugallery.com/webdata/product/32379/view1/large__dsc2395h.jpg</t>
+  </si>
+  <si>
+    <t>http://www.ugallery.com/webdata/product/43981/view1/large_enigmaside.jpg</t>
+  </si>
+  <si>
+    <t>http://www.ugallery.com/webdata/product/43980/view1/large_whatliesbeneathviside.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/40349/Images/Large_red.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/45751/Images/Large_imgp1400.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/42648/Images/Large_16x24ColorsOfBulldog1.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/45351/Images/large_lovesongs0743.jpg</t>
+  </si>
+  <si>
+    <t>http://www.ugallery.com/webdata/Product/44651/Images/Large_400.yellowfieldwithmesa.jpg</t>
+  </si>
+  <si>
+    <t>http://www.ugallery.com/webdata/Product/43677/Images/Large_Main.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/38259/Images/Large_Mountain_Dance.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://s-media-cache-ak0.pinimg.com/736x/e0/74/38/e07438ffa3db2fd3730efd020a89b84d.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://s-media-cache-ak0.pinimg.com/736x/dc/70/fb/dc70fbaaef98a4fee4b8fd68109d129b.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://product-images.highwire.com/7487644/cant02.jpg (212KB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://ecx.images-amazon.com/images/I/91T6TssKyWL._SY500_.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://s-media-cache-ak0.pinimg.com/736x/c1/6a/29/c16a29e76b9943f54e41ceaa056110e7.jpg</t>
+  </si>
+  <si>
+    <t>http://static.ugallery.com/webdata/Product/43860/Images/Large_craterlakephantomshipislandsunset.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ugallery.com/webdata/Product/42754/images/list_Coastal_Plain_40x40_Ugallery.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/45408/Images/Large_iii.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://s-media-cache-ak0.pinimg.com/736x/13/23/53/132353ad96510acd0906f0dbe09fb9b9.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/43295/Images/Large_pathtothelakeupdate.jpg</t>
+  </si>
+  <si>
+    <t>http://st.hzcdn.com/simgs/13f107ce0164ddc1_4-4868/contemporary-artwork.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/42831/Images/Large_peacock.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/41772/Images/Large_The_Amputee.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/40336/Images/Large_deaths_head_(full).jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/45755/Images/Large_bruges.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://s-media-cache-ak0.pinimg.com/236x/67/fa/29/67fa297005e0dc8e620ef161289acc7a.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ugallery.com/webdata/product/30689/view3/large_patterson_heather_luz_detail3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ugallery.com/webdata/Product/39734/Images/Large_vessel2_rees.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/39731/Images/Large_plantedseed_rees.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://www.ugallery.com/webdata/product/44357/view2/large_airmailwall.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/45321/Images/Large_hopeisathingwithfeathersmain.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.ugallery.com/webdata/product/42883/view2/large_img_5458.jpg </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://static.ugallery.com/webdata/Product/39847/Images/Large_memory_ring_mini_full.jpg</t>
+  </si>
+  <si>
+    <t>http://www.alexandreev.com/sites/default/files/styles/work_portrait/public/artworks/Vesper.jpg?itok=xkVaQrcH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://static.ugallery.com/webdata/Product/28729/Images/Large_Under_the_rain.jpg </t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Caching</t>
+  </si>
+  <si>
+    <t>Content-Type</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>HTTP</t>
+  </si>
+  <si>
+    <t>localhost:49155</t>
+  </si>
+  <si>
+    <t>/vshub/2f587bd2488b44219167715f6bc3f178/DataWarehouseModule/dataWarehouse/getStatus/</t>
+  </si>
+  <si>
+    <t>application/json; charset=utf-8</t>
+  </si>
+  <si>
+    <t>scriptedsandbox64:21488</t>
+  </si>
 </sst>
 </file>
 
@@ -1026,7 +1221,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,6 +1268,11 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555459"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1129,7 +1329,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1154,6 +1354,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1470,18 +1685,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView topLeftCell="F29" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="18" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
@@ -1525,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="18" customFormat="1">
       <c r="A2" s="18" t="s">
         <v>36</v>
       </c>
@@ -1560,7 +1775,7 @@
         <v>263</v>
       </c>
       <c r="L2" s="19">
-        <f>M2*0.63</f>
+        <f t="shared" ref="L2:L33" si="0">M2*0.63</f>
         <v>945</v>
       </c>
       <c r="M2" s="20">
@@ -1569,8 +1784,11 @@
       <c r="N2" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="25" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="18" customFormat="1" ht="16.2" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>104</v>
       </c>
@@ -1605,7 +1823,7 @@
         <v>265</v>
       </c>
       <c r="L3" s="19">
-        <f>M3*0.63</f>
+        <f t="shared" si="0"/>
         <v>945</v>
       </c>
       <c r="M3" s="20">
@@ -1614,8 +1832,11 @@
       <c r="N3" s="18" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O3" s="25" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="18" customFormat="1">
       <c r="A4" s="18" t="s">
         <v>108</v>
       </c>
@@ -1650,7 +1871,7 @@
         <v>265</v>
       </c>
       <c r="L4" s="19">
-        <f>M4*0.63</f>
+        <f t="shared" si="0"/>
         <v>976.5</v>
       </c>
       <c r="M4" s="12">
@@ -1659,8 +1880,11 @@
       <c r="N4" s="7" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O4" s="25" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="18" customFormat="1">
       <c r="A5" s="18" t="s">
         <v>150</v>
       </c>
@@ -1692,7 +1916,7 @@
         <v>266</v>
       </c>
       <c r="L5" s="19">
-        <f>M5*0.63</f>
+        <f t="shared" si="0"/>
         <v>425.25</v>
       </c>
       <c r="M5" s="12">
@@ -1701,8 +1925,11 @@
       <c r="N5" s="18" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O5" s="24" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="18" customFormat="1">
       <c r="A6" s="18" t="s">
         <v>163</v>
       </c>
@@ -1734,7 +1961,7 @@
         <v>265</v>
       </c>
       <c r="L6" s="19">
-        <f>M6*0.63</f>
+        <f t="shared" si="0"/>
         <v>346.5</v>
       </c>
       <c r="M6" s="12">
@@ -1743,8 +1970,11 @@
       <c r="N6" s="18" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O6" s="24" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="18" customFormat="1">
       <c r="A7" s="18" t="s">
         <v>118</v>
       </c>
@@ -1779,7 +2009,7 @@
         <v>264</v>
       </c>
       <c r="L7" s="19">
-        <f>M7*0.63</f>
+        <f t="shared" si="0"/>
         <v>1165.5</v>
       </c>
       <c r="M7" s="12">
@@ -1788,8 +2018,11 @@
       <c r="N7" s="18" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="24" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="18" customFormat="1">
       <c r="A8" s="18" t="s">
         <v>124</v>
       </c>
@@ -1824,7 +2057,7 @@
         <v>264</v>
       </c>
       <c r="L8" s="19">
-        <f>M8*0.63</f>
+        <f t="shared" si="0"/>
         <v>1039.5</v>
       </c>
       <c r="M8" s="12">
@@ -1833,8 +2066,11 @@
       <c r="N8" s="18" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O8" s="24" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="18" customFormat="1">
       <c r="A9" s="18" t="s">
         <v>222</v>
       </c>
@@ -1866,7 +2102,7 @@
         <v>266</v>
       </c>
       <c r="L9" s="19">
-        <f>M9*0.63</f>
+        <f t="shared" si="0"/>
         <v>220.5</v>
       </c>
       <c r="M9" s="20">
@@ -1875,8 +2111,11 @@
       <c r="N9" s="18" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O9" s="24" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="18" customFormat="1">
       <c r="A10" s="18" t="s">
         <v>187</v>
       </c>
@@ -1911,7 +2150,7 @@
         <v>264</v>
       </c>
       <c r="L10" s="19">
-        <f>M10*0.63</f>
+        <f t="shared" si="0"/>
         <v>78.75</v>
       </c>
       <c r="M10" s="20">
@@ -1920,8 +2159,11 @@
       <c r="N10" s="18" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O10" s="24" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="18" customFormat="1">
       <c r="A11" s="18" t="s">
         <v>190</v>
       </c>
@@ -1956,7 +2198,7 @@
         <v>264</v>
       </c>
       <c r="L11" s="19">
-        <f>M11*0.63</f>
+        <f t="shared" si="0"/>
         <v>78.75</v>
       </c>
       <c r="M11" s="20">
@@ -1965,8 +2207,11 @@
       <c r="N11" s="18" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O11" s="25" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="18" customFormat="1">
       <c r="A12" s="18" t="s">
         <v>50</v>
       </c>
@@ -1998,7 +2243,7 @@
         <v>265</v>
       </c>
       <c r="L12" s="19">
-        <f>M12*0.63</f>
+        <f t="shared" si="0"/>
         <v>141.75</v>
       </c>
       <c r="M12" s="20">
@@ -2007,8 +2252,11 @@
       <c r="N12" s="18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="24" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="18" customFormat="1">
       <c r="A13" s="18" t="s">
         <v>256</v>
       </c>
@@ -2040,7 +2288,7 @@
         <v>266</v>
       </c>
       <c r="L13" s="19">
-        <f>M13*0.63</f>
+        <f t="shared" si="0"/>
         <v>645.75</v>
       </c>
       <c r="M13" s="20">
@@ -2049,8 +2297,11 @@
       <c r="N13" s="18" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="24" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="18" customFormat="1">
       <c r="A14" s="18" t="s">
         <v>74</v>
       </c>
@@ -2083,7 +2334,7 @@
         <v>266</v>
       </c>
       <c r="L14" s="19">
-        <f>M14*0.63</f>
+        <f t="shared" si="0"/>
         <v>1055.25</v>
       </c>
       <c r="M14" s="20">
@@ -2092,8 +2343,11 @@
       <c r="N14" s="18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="24" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="18" customFormat="1">
       <c r="A15" s="18" t="s">
         <v>242</v>
       </c>
@@ -2125,7 +2379,7 @@
         <v>266</v>
       </c>
       <c r="L15" s="19">
-        <f>M15*0.63</f>
+        <f t="shared" si="0"/>
         <v>378</v>
       </c>
       <c r="M15" s="20">
@@ -2134,8 +2388,11 @@
       <c r="N15" s="18" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O15" s="24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="18" customFormat="1">
       <c r="A16" s="18" t="s">
         <v>132</v>
       </c>
@@ -2170,7 +2427,7 @@
         <v>265</v>
       </c>
       <c r="L16" s="19">
-        <f>M16*0.63</f>
+        <f t="shared" si="0"/>
         <v>173.25</v>
       </c>
       <c r="M16" s="12">
@@ -2179,8 +2436,11 @@
       <c r="N16" s="18" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O16" s="25" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="18" customFormat="1">
       <c r="A17" s="18" t="s">
         <v>154</v>
       </c>
@@ -2212,7 +2472,7 @@
         <v>263</v>
       </c>
       <c r="L17" s="19">
-        <f>M17*0.63</f>
+        <f t="shared" si="0"/>
         <v>1008</v>
       </c>
       <c r="M17" s="12">
@@ -2221,8 +2481,11 @@
       <c r="N17" s="18" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O17" s="24" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="18" customFormat="1">
       <c r="A18" s="18" t="s">
         <v>44</v>
       </c>
@@ -2254,7 +2517,7 @@
         <v>264</v>
       </c>
       <c r="L18" s="19">
-        <f>M18*0.63</f>
+        <f t="shared" si="0"/>
         <v>315</v>
       </c>
       <c r="M18" s="20">
@@ -2263,8 +2526,11 @@
       <c r="N18" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O18" s="24" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="18" customFormat="1">
       <c r="A19" s="18" t="s">
         <v>176</v>
       </c>
@@ -2296,7 +2562,7 @@
         <v>266</v>
       </c>
       <c r="L19" s="19">
-        <f>M19*0.63</f>
+        <f t="shared" si="0"/>
         <v>252</v>
       </c>
       <c r="M19" s="20">
@@ -2305,8 +2571,11 @@
       <c r="N19" s="18" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O19" s="24" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="18" customFormat="1">
       <c r="A20" s="18" t="s">
         <v>248</v>
       </c>
@@ -2338,7 +2607,7 @@
         <v>263</v>
       </c>
       <c r="L20" s="19">
-        <f>M20*0.63</f>
+        <f t="shared" si="0"/>
         <v>929.25</v>
       </c>
       <c r="M20" s="20">
@@ -2347,8 +2616,11 @@
       <c r="N20" s="18" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O20" s="24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="18" customFormat="1">
       <c r="A21" s="18" t="s">
         <v>112</v>
       </c>
@@ -2383,7 +2655,7 @@
         <v>266</v>
       </c>
       <c r="L21" s="19">
-        <f>M21*0.63</f>
+        <f t="shared" si="0"/>
         <v>315</v>
       </c>
       <c r="M21" s="12">
@@ -2392,8 +2664,11 @@
       <c r="N21" s="18" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O21" s="24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="18" customFormat="1">
       <c r="A22" s="18" t="s">
         <v>100</v>
       </c>
@@ -2426,7 +2701,7 @@
         <v>264</v>
       </c>
       <c r="L22" s="19">
-        <f>M22*0.63</f>
+        <f t="shared" si="0"/>
         <v>551.25</v>
       </c>
       <c r="M22" s="20">
@@ -2435,8 +2710,11 @@
       <c r="N22" s="18" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O22" s="24" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="18" customFormat="1">
       <c r="A23" s="18" t="s">
         <v>139</v>
       </c>
@@ -2468,7 +2746,7 @@
         <v>266</v>
       </c>
       <c r="L23" s="19">
-        <f>M23*0.63</f>
+        <f t="shared" si="0"/>
         <v>677.25</v>
       </c>
       <c r="M23" s="12">
@@ -2477,8 +2755,11 @@
       <c r="N23" s="18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O23" s="24" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" s="18" customFormat="1">
       <c r="A24" s="18" t="s">
         <v>147</v>
       </c>
@@ -2510,7 +2791,7 @@
         <v>264</v>
       </c>
       <c r="L24" s="19">
-        <f>M24*0.63</f>
+        <f t="shared" si="0"/>
         <v>661.5</v>
       </c>
       <c r="M24" s="12">
@@ -2519,8 +2800,11 @@
       <c r="N24" s="18" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O24" s="24" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="18" customFormat="1">
       <c r="A25" s="18" t="s">
         <v>233</v>
       </c>
@@ -2552,7 +2836,7 @@
         <v>266</v>
       </c>
       <c r="L25" s="19">
-        <f>M25*0.63</f>
+        <f t="shared" si="0"/>
         <v>252</v>
       </c>
       <c r="M25" s="20">
@@ -2561,8 +2845,11 @@
       <c r="N25" s="18" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O25" s="24" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="18" customFormat="1">
       <c r="A26" s="18" t="s">
         <v>238</v>
       </c>
@@ -2594,7 +2881,7 @@
         <v>264</v>
       </c>
       <c r="L26" s="19">
-        <f>M26*0.63</f>
+        <f t="shared" si="0"/>
         <v>378</v>
       </c>
       <c r="M26" s="20">
@@ -2603,8 +2890,11 @@
       <c r="N26" s="18" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O26" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="18" customFormat="1">
       <c r="A27" s="18" t="s">
         <v>167</v>
       </c>
@@ -2636,7 +2926,7 @@
         <v>266</v>
       </c>
       <c r="L27" s="19">
-        <f>M27*0.63</f>
+        <f t="shared" si="0"/>
         <v>567</v>
       </c>
       <c r="M27" s="12">
@@ -2645,8 +2935,11 @@
       <c r="N27" s="18" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O27" s="25" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" s="18" customFormat="1">
       <c r="A28" s="18" t="s">
         <v>143</v>
       </c>
@@ -2678,7 +2971,7 @@
         <v>264</v>
       </c>
       <c r="L28" s="19">
-        <f>M28*0.63</f>
+        <f t="shared" si="0"/>
         <v>346.5</v>
       </c>
       <c r="M28" s="12">
@@ -2687,8 +2980,11 @@
       <c r="N28" s="18" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O28" s="24" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="18" customFormat="1">
       <c r="A29" s="18" t="s">
         <v>95</v>
       </c>
@@ -2721,7 +3017,7 @@
         <v>263</v>
       </c>
       <c r="L29" s="19">
-        <f>M29*0.63</f>
+        <f t="shared" si="0"/>
         <v>645.75</v>
       </c>
       <c r="M29" s="20">
@@ -2730,8 +3026,11 @@
       <c r="N29" s="18" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O29" s="24" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="18" customFormat="1">
       <c r="A30" s="18" t="s">
         <v>207</v>
       </c>
@@ -2763,7 +3062,7 @@
         <v>265</v>
       </c>
       <c r="L30" s="19">
-        <f>M30*0.63</f>
+        <f t="shared" si="0"/>
         <v>299.25</v>
       </c>
       <c r="M30" s="20">
@@ -2772,8 +3071,11 @@
       <c r="N30" s="18" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O30" s="24" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="18" customFormat="1">
       <c r="A31" s="18" t="s">
         <v>172</v>
       </c>
@@ -2805,7 +3107,7 @@
         <v>266</v>
       </c>
       <c r="L31" s="19">
-        <f>M31*0.63</f>
+        <f t="shared" si="0"/>
         <v>141.75</v>
       </c>
       <c r="M31" s="20">
@@ -2814,8 +3116,11 @@
       <c r="N31" s="18" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O31" s="24" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="18" customFormat="1">
       <c r="A32" s="18" t="s">
         <v>90</v>
       </c>
@@ -2848,7 +3153,7 @@
         <v>263</v>
       </c>
       <c r="L32" s="19">
-        <f>M32*0.63</f>
+        <f t="shared" si="0"/>
         <v>913.5</v>
       </c>
       <c r="M32" s="20">
@@ -2857,8 +3162,11 @@
       <c r="N32" s="18" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O32" s="24" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="18" customFormat="1">
       <c r="A33" s="18" t="s">
         <v>69</v>
       </c>
@@ -2891,7 +3199,7 @@
         <v>266</v>
       </c>
       <c r="L33" s="19">
-        <f>M33*0.63</f>
+        <f t="shared" si="0"/>
         <v>567</v>
       </c>
       <c r="M33" s="20">
@@ -2900,8 +3208,11 @@
       <c r="N33" s="18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O33" s="24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="18" customFormat="1">
       <c r="A34" s="18" t="s">
         <v>158</v>
       </c>
@@ -2933,7 +3244,7 @@
         <v>265</v>
       </c>
       <c r="L34" s="19">
-        <f>M34*0.63</f>
+        <f t="shared" ref="L34:L65" si="1">M34*0.63</f>
         <v>378</v>
       </c>
       <c r="M34" s="12">
@@ -2942,8 +3253,11 @@
       <c r="N34" s="18" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O34" s="24" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="18" customFormat="1">
       <c r="A35" s="18" t="s">
         <v>179</v>
       </c>
@@ -2978,7 +3292,7 @@
         <v>264</v>
       </c>
       <c r="L35" s="19">
-        <f>M35*0.63</f>
+        <f t="shared" si="1"/>
         <v>78.75</v>
       </c>
       <c r="M35" s="20">
@@ -2987,8 +3301,11 @@
       <c r="N35" s="18" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O35" s="24" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" s="18" customFormat="1">
       <c r="A36" s="18" t="s">
         <v>252</v>
       </c>
@@ -3020,7 +3337,7 @@
         <v>265</v>
       </c>
       <c r="L36" s="19">
-        <f>M36*0.63</f>
+        <f t="shared" si="1"/>
         <v>488.25</v>
       </c>
       <c r="M36" s="20">
@@ -3029,8 +3346,11 @@
       <c r="N36" s="18" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O36" s="24" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" s="18" customFormat="1">
       <c r="A37" s="18" t="s">
         <v>199</v>
       </c>
@@ -3062,7 +3382,7 @@
         <v>265</v>
       </c>
       <c r="L37" s="19">
-        <f>M37*0.63</f>
+        <f t="shared" si="1"/>
         <v>551.25</v>
       </c>
       <c r="M37" s="20">
@@ -3071,8 +3391,11 @@
       <c r="N37" s="18" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O37" s="24" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" s="18" customFormat="1">
       <c r="A38" s="18" t="s">
         <v>203</v>
       </c>
@@ -3104,7 +3427,7 @@
         <v>265</v>
       </c>
       <c r="L38" s="19">
-        <f>M38*0.63</f>
+        <f t="shared" si="1"/>
         <v>393.75</v>
       </c>
       <c r="M38" s="20">
@@ -3113,8 +3436,11 @@
       <c r="N38" s="18" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O38" s="24" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="18" customFormat="1">
       <c r="A39" s="18" t="s">
         <v>30</v>
       </c>
@@ -3149,7 +3475,7 @@
         <v>263</v>
       </c>
       <c r="L39" s="19">
-        <f>M39*0.63</f>
+        <f t="shared" si="1"/>
         <v>929.25</v>
       </c>
       <c r="M39" s="20">
@@ -3158,8 +3484,11 @@
       <c r="N39" s="18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O39" s="24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" s="18" customFormat="1">
       <c r="A40" s="18" t="s">
         <v>79</v>
       </c>
@@ -3192,7 +3521,7 @@
         <v>263</v>
       </c>
       <c r="L40" s="19">
-        <f>M40*0.63</f>
+        <f t="shared" si="1"/>
         <v>330.75</v>
       </c>
       <c r="M40" s="20">
@@ -3201,8 +3530,11 @@
       <c r="N40" s="18" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O40" s="24" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" s="18" customFormat="1">
       <c r="A41" s="18" t="s">
         <v>57</v>
       </c>
@@ -3234,7 +3566,7 @@
         <v>263</v>
       </c>
       <c r="L41" s="19">
-        <f>M41*0.63</f>
+        <f t="shared" si="1"/>
         <v>220.5</v>
       </c>
       <c r="M41" s="20">
@@ -3243,8 +3575,11 @@
       <c r="N41" s="18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O41" s="24" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" s="18" customFormat="1">
       <c r="A42" s="18" t="s">
         <v>66</v>
       </c>
@@ -3279,7 +3614,7 @@
         <v>264</v>
       </c>
       <c r="L42" s="19">
-        <f>M42*0.63</f>
+        <f t="shared" si="1"/>
         <v>220.5</v>
       </c>
       <c r="M42" s="20">
@@ -3288,8 +3623,11 @@
       <c r="N42" s="18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O42" s="24" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" s="18" customFormat="1">
       <c r="A43" s="18" t="s">
         <v>127</v>
       </c>
@@ -3324,7 +3662,7 @@
         <v>263</v>
       </c>
       <c r="L43" s="19">
-        <f>M43*0.63</f>
+        <f t="shared" si="1"/>
         <v>1527.75</v>
       </c>
       <c r="M43" s="12">
@@ -3333,8 +3671,11 @@
       <c r="N43" s="18" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O43" s="24" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" s="18" customFormat="1">
       <c r="A44" s="18" t="s">
         <v>193</v>
       </c>
@@ -3366,7 +3707,7 @@
         <v>264</v>
       </c>
       <c r="L44" s="19">
-        <f>M44*0.63</f>
+        <f t="shared" si="1"/>
         <v>283.5</v>
       </c>
       <c r="M44" s="20">
@@ -3375,8 +3716,11 @@
       <c r="N44" s="18" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O44" s="24" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" s="18" customFormat="1">
       <c r="A45" s="18" t="s">
         <v>183</v>
       </c>
@@ -3411,7 +3755,7 @@
         <v>264</v>
       </c>
       <c r="L45" s="19">
-        <f>M45*0.63</f>
+        <f t="shared" si="1"/>
         <v>126</v>
       </c>
       <c r="M45" s="20">
@@ -3420,8 +3764,11 @@
       <c r="N45" s="18" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O45" s="24" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" s="18" customFormat="1">
       <c r="A46" s="18" t="s">
         <v>211</v>
       </c>
@@ -3453,7 +3800,7 @@
         <v>263</v>
       </c>
       <c r="L46" s="19">
-        <f>M46*0.63</f>
+        <f t="shared" si="1"/>
         <v>299.25</v>
       </c>
       <c r="M46" s="20">
@@ -3462,8 +3809,11 @@
       <c r="N46" s="18" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O46" s="24" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" s="18" customFormat="1">
       <c r="A47" s="18" t="s">
         <v>65</v>
       </c>
@@ -3495,7 +3845,7 @@
         <v>266</v>
       </c>
       <c r="L47" s="19">
-        <f>M47*0.63</f>
+        <f t="shared" si="1"/>
         <v>1779.75</v>
       </c>
       <c r="M47" s="20">
@@ -3504,8 +3854,11 @@
       <c r="N47" s="18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O47" s="24" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>227</v>
       </c>
@@ -3537,7 +3890,7 @@
         <v>266</v>
       </c>
       <c r="L48" s="13">
-        <f>M48*0.63</f>
+        <f t="shared" si="1"/>
         <v>173.25</v>
       </c>
       <c r="M48" s="8">
@@ -3546,8 +3899,11 @@
       <c r="N48" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O48" s="24" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="18" customFormat="1">
       <c r="A49" s="18" t="s">
         <v>217</v>
       </c>
@@ -3579,7 +3935,7 @@
         <v>263</v>
       </c>
       <c r="L49" s="19">
-        <f>M49*0.63</f>
+        <f t="shared" si="1"/>
         <v>378</v>
       </c>
       <c r="M49" s="20">
@@ -3588,8 +3944,11 @@
       <c r="N49" s="18" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O49" s="24" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" s="18" t="s">
         <v>85</v>
       </c>
@@ -3622,7 +3981,7 @@
         <v>263</v>
       </c>
       <c r="L50" s="19">
-        <f>M50*0.63</f>
+        <f t="shared" si="1"/>
         <v>298.62</v>
       </c>
       <c r="M50" s="20">
@@ -3631,33 +3990,44 @@
       <c r="N50" s="18" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O50" s="24" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="I51" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:N51">
     <sortCondition ref="B1"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="O11" r:id="rId1"/>
+    <hyperlink ref="O16" r:id="rId2"/>
+    <hyperlink ref="O27" r:id="rId3"/>
+    <hyperlink ref="O2" r:id="rId4"/>
+    <hyperlink ref="O3" r:id="rId5"/>
+    <hyperlink ref="O4" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="10" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3689,7 +4059,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3721,7 +4091,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3753,7 +4123,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3785,7 +4155,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3817,7 +4187,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3849,7 +4219,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3881,7 +4251,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3913,7 +4283,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3945,7 +4315,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3977,7 +4347,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4009,7 +4379,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4041,7 +4411,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4073,29 +4443,93 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12">
       <c r="C17" s="7"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12">
       <c r="F18" s="15"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="28.8">
+      <c r="B19" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>377</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="H19" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>382</v>
+      </c>
+      <c r="J19" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="57.6">
+      <c r="B20" s="27">
+        <v>6735</v>
+      </c>
+      <c r="C20" s="27">
+        <v>201</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="G20" s="28">
+        <v>1338</v>
+      </c>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27" t="s">
+        <v>389</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+    </row>
+    <row r="21" spans="2:12">
       <c r="F21" s="14"/>
     </row>
   </sheetData>
@@ -4107,18 +4541,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="4" width="22.77734375" customWidth="1"/>
     <col min="5" max="5" width="50.44140625" customWidth="1"/>
     <col min="6" max="8" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -4144,7 +4578,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>312</v>
       </c>
@@ -4170,7 +4604,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>316</v>
       </c>
@@ -4196,7 +4630,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -4222,7 +4656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>318</v>
       </c>
@@ -4248,42 +4682,42 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="7"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>